<commit_message>
Atualização da macro para dar refresh nas gregas e código salvando os arquivos nos destinos corretos
</commit_message>
<xml_diff>
--- a/data/plan_base.xlsx
+++ b/data/plan_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d54ad363d82ba0fc/Documentos/GitHub/padulla/black_scholes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:40009_{48EDCEF4-549A-4538-A985-A07D60102E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DA9F89D3-1A72-4573-A46D-EF85C5F9B1A9}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:40009_{48EDCEF4-549A-4538-A985-A07D60102E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F9E01C30-510B-4E45-936C-3275F6FA2960}"/>
   <bookViews>
-    <workbookView xWindow="32865" yWindow="2595" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32520" yWindow="2250" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão da linha para pegar o dado no excel
</commit_message>
<xml_diff>
--- a/data/plan_base.xlsx
+++ b/data/plan_base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d54ad363d82ba0fc/Documentos/GitHub/padulla/black_scholes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="13_ncr:40009_{48EDCEF4-549A-4538-A985-A07D60102E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7A9D176A-3CA6-44B9-8EF8-E7AC3274CB9A}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:40009_{48EDCEF4-549A-4538-A985-A07D60102E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{503FB950-5965-4D80-8067-B12CF35C90DC}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2460" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>

</xml_diff>